<commit_message>
Results from July 15, 2020 05:41:04 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-15.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-15.xlsx
@@ -569,13 +569,13 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="C3" t="n">
-        <v>21067</v>
+        <v>21546</v>
       </c>
       <c r="D3" t="n">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="E3" t="n">
         <v>464</v>
@@ -880,19 +880,19 @@
         <v>44027</v>
       </c>
       <c r="C9" t="n">
-        <v>29733</v>
+        <v>30297</v>
       </c>
       <c r="D9" t="n">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="E9" t="n">
-        <v>6283</v>
+        <v>6444</v>
       </c>
       <c r="F9" t="n">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="G9" t="n">
-        <v>24.74</v>
+        <v>24.63</v>
       </c>
       <c r="H9" t="n">
         <v>26.13</v>
@@ -904,10 +904,10 @@
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>25396</v>
+        <v>26159</v>
       </c>
       <c r="L9" t="n">
-        <v>310</v>
+        <v>333</v>
       </c>
       <c r="M9" t="n">
         <v>460970</v>
@@ -928,25 +928,25 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="C10" t="n">
-        <v>20887</v>
+        <v>21446</v>
       </c>
       <c r="D10" t="n">
-        <v>436</v>
+        <v>448</v>
       </c>
       <c r="E10" t="n">
-        <v>768</v>
+        <v>786</v>
       </c>
       <c r="F10" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G10" t="n">
-        <v>4.66</v>
+        <v>4.67</v>
       </c>
       <c r="H10" t="n">
-        <v>3.75</v>
+        <v>4.14</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
@@ -955,10 +955,10 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>16473</v>
+        <v>16838</v>
       </c>
       <c r="L10" t="n">
-        <v>427</v>
+        <v>435</v>
       </c>
       <c r="M10" t="n">
         <v>166412</v>
@@ -1649,25 +1649,25 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="C25" t="n">
-        <v>21717</v>
+        <v>21979</v>
       </c>
       <c r="D25" t="n">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="E25" t="n">
-        <v>1275</v>
+        <v>1286</v>
       </c>
       <c r="F25" t="n">
         <v>22</v>
       </c>
       <c r="G25" t="n">
-        <v>7.63</v>
+        <v>7.61</v>
       </c>
       <c r="H25" t="n">
-        <v>7.97</v>
+        <v>8</v>
       </c>
       <c r="I25" t="b">
         <v>0</v>
@@ -1676,10 +1676,10 @@
         <v>1</v>
       </c>
       <c r="K25" t="n">
-        <v>16719</v>
+        <v>16891</v>
       </c>
       <c r="L25" t="n">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="M25" t="n">
         <v>90860</v>
@@ -1746,21 +1746,39 @@
           <t>California</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
+      <c r="B27" s="2" t="n">
+        <v>44026</v>
+      </c>
+      <c r="C27" t="n">
+        <v>347634</v>
+      </c>
+      <c r="D27" t="n">
+        <v>7164</v>
+      </c>
+      <c r="E27" t="n">
+        <v>9697</v>
+      </c>
+      <c r="F27" t="n">
+        <v>621</v>
+      </c>
+      <c r="G27" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="H27" t="n">
+        <v>8.800000000000001</v>
+      </c>
       <c r="I27" t="b">
         <v>0</v>
       </c>
       <c r="J27" t="b">
-        <v>0</v>
-      </c>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K27" t="n">
+        <v>223576</v>
+      </c>
+      <c r="L27" t="n">
+        <v>7038</v>
+      </c>
       <c r="M27" t="n">
         <v>2267875</v>
       </c>
@@ -1769,7 +1787,7 @@
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>An error occurred. ... ConnectionError(ProtocolError('Connection aborted.', ConnectionResetError(104, 'Connection reset by peer')))</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
@@ -1976,25 +1994,25 @@
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="C32" t="n">
-        <v>42304</v>
+        <v>43046</v>
       </c>
       <c r="D32" t="n">
-        <v>1404</v>
+        <v>1421</v>
       </c>
       <c r="E32" t="n">
-        <v>1618</v>
+        <v>1649</v>
       </c>
       <c r="F32" t="n">
         <v>48</v>
       </c>
       <c r="G32" t="n">
-        <v>5.44</v>
+        <v>5.45</v>
       </c>
       <c r="H32" t="n">
-        <v>3.58</v>
+        <v>3.53</v>
       </c>
       <c r="I32" t="b">
         <v>0</v>
@@ -2003,10 +2021,10 @@
         <v>0</v>
       </c>
       <c r="K32" t="n">
-        <v>29767</v>
+        <v>30278</v>
       </c>
       <c r="L32" t="n">
-        <v>1339</v>
+        <v>1359</v>
       </c>
       <c r="M32" t="n">
         <v>269854</v>
@@ -2169,22 +2187,22 @@
         <v>44027</v>
       </c>
       <c r="C36" t="n">
-        <v>36297</v>
+        <v>36322</v>
       </c>
       <c r="D36" t="n">
-        <v>767</v>
+        <v>772</v>
       </c>
       <c r="E36" t="n">
-        <v>3102</v>
+        <v>3104</v>
       </c>
       <c r="F36" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G36" t="n">
         <v>8.550000000000001</v>
       </c>
       <c r="H36" t="n">
-        <v>4.69</v>
+        <v>4.79</v>
       </c>
       <c r="I36" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Results from July 15, 2020 07:37:50 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-15.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-15.xlsx
@@ -1210,25 +1210,25 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44025</v>
+        <v>44026</v>
       </c>
       <c r="C16" t="n">
-        <v>140307</v>
+        <v>143009</v>
       </c>
       <c r="D16" t="n">
-        <v>3894</v>
+        <v>3936</v>
       </c>
       <c r="E16" t="n">
-        <v>3737</v>
+        <v>3818</v>
       </c>
       <c r="F16" t="n">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="G16" t="n">
-        <v>4.69</v>
+        <v>4.7</v>
       </c>
       <c r="H16" t="n">
-        <v>10.8</v>
+        <v>10.74</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
@@ -1237,10 +1237,10 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>79721</v>
+        <v>81305</v>
       </c>
       <c r="L16" t="n">
-        <v>3619</v>
+        <v>3658</v>
       </c>
       <c r="M16" t="n">
         <v>823987</v>
@@ -1753,7 +1753,7 @@
         <v>347634</v>
       </c>
       <c r="D27" t="n">
-        <v>7164</v>
+        <v>7227</v>
       </c>
       <c r="E27" t="n">
         <v>9697</v>
@@ -1762,16 +1762,16 @@
         <v>621</v>
       </c>
       <c r="G27" t="n">
-        <v>4.3</v>
+        <v>4.34</v>
       </c>
       <c r="H27" t="n">
-        <v>8.800000000000001</v>
+        <v>8.82</v>
       </c>
       <c r="I27" t="b">
         <v>0</v>
       </c>
       <c r="J27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K27" t="n">
         <v>223576</v>
@@ -2187,7 +2187,7 @@
         <v>44027</v>
       </c>
       <c r="C36" t="n">
-        <v>36322</v>
+        <v>36324</v>
       </c>
       <c r="D36" t="n">
         <v>772</v>

</xml_diff>

<commit_message>
Results from July 15, 2020 07:45:49 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-15.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-15.xlsx
@@ -2187,19 +2187,19 @@
         <v>44027</v>
       </c>
       <c r="C36" t="n">
-        <v>36324</v>
+        <v>36408</v>
       </c>
       <c r="D36" t="n">
         <v>772</v>
       </c>
       <c r="E36" t="n">
-        <v>3104</v>
+        <v>3110</v>
       </c>
       <c r="F36" t="n">
         <v>37</v>
       </c>
       <c r="G36" t="n">
-        <v>8.550000000000001</v>
+        <v>8.539999999999999</v>
       </c>
       <c r="H36" t="n">
         <v>4.79</v>

</xml_diff>